<commit_message>
add pivot functionality with Streamlit interface and Excel file support
</commit_message>
<xml_diff>
--- a/python/example_timetable.xlsx
+++ b/python/example_timetable.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\matu\work\ToDo\convex\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D9F6A9-4A03-44AB-8DDA-38D948C899E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF580C2-9FDD-4800-871C-04CEEF76CFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1425" windowWidth="12795" windowHeight="10275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="setting_for_highlight" sheetId="3" r:id="rId2"/>
+    <sheet name="setting_for_pivotea" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="69">
   <si>
     <t>semester</t>
     <phoneticPr fontId="1"/>
@@ -348,6 +349,30 @@
   </si>
   <si>
     <t>sky</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>split</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>col</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>row</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>item</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>position</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -400,10 +425,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -686,11 +712,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -3852,9 +3876,9 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3947,4 +3971,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9046A511-97EC-4D98-BE01-3C6EF998885C}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>